<commit_message>
Modified excel file with notes for problem 125.
</commit_message>
<xml_diff>
--- a/problem_notes.xlsx
+++ b/problem_notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13391340-D714-4974-9B8E-3654D69522C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6DC333-957F-4CEC-8937-4E9207E35878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31275" yWindow="825" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
+    <workbookView xWindow="31065" yWindow="1260" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Category</t>
   </si>
@@ -45,6 +45,15 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Two Pointers</t>
+  </si>
+  <si>
+    <t>125 - Valid Palindrome</t>
+  </si>
+  <si>
+    <t>Python strings have several methods to check for their type of contents. Start a pointer at each side of the string and check for equality.</t>
   </si>
 </sst>
 </file>
@@ -60,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,8 +95,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -416,23 +435,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041B7148-3DCA-4078-893C-34A3490F6593}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="3" max="3" width="139.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished one solution to problem 125 and updated problem table
</commit_message>
<xml_diff>
--- a/problem_notes.xlsx
+++ b/problem_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6DC333-957F-4CEC-8937-4E9207E35878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130EAD5D-ABBE-4046-8193-7C5192190A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31065" yWindow="1260" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
   </bookViews>
@@ -53,7 +53,8 @@
     <t>125 - Valid Palindrome</t>
   </si>
   <si>
-    <t>Python strings have several methods to check for their type of contents. Start a pointer at each side of the string and check for equality.</t>
+    <t>Python strings have several methods to check for their type of contents. 1. Find logic in the problem. Palindromes read the same both ways, reverse the string.
+2. Start a pointer at each side of the string and check for equality.</t>
   </si>
 </sst>
 </file>
@@ -95,12 +96,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,14 +447,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="3" max="3" width="139.7109375" customWidth="1"/>
+    <col min="3" max="3" width="138.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -459,14 +468,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished problem 125 and explained general ideas in the problems table.
</commit_message>
<xml_diff>
--- a/problem_notes.xlsx
+++ b/problem_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{130EAD5D-ABBE-4046-8193-7C5192190A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E5D8F-03F9-4D4D-BA19-94E97E227534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31065" yWindow="1260" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
   </bookViews>
@@ -54,7 +54,7 @@
   </si>
   <si>
     <t>Python strings have several methods to check for their type of contents. 1. Find logic in the problem. Palindromes read the same both ways, reverse the string.
-2. Start a pointer at each side of the string and check for equality.</t>
+2. Start a pointer at each side of the string, use an alphanumeric validation function, and move the pointers if they are not alphanumeric.</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added notes to a previous problem and for the one I'm currently working on.
</commit_message>
<xml_diff>
--- a/problem_notes.xlsx
+++ b/problem_notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704E5D8F-03F9-4D4D-BA19-94E97E227534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5E502A-8900-4280-9774-8977AD5A8B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31065" yWindow="1260" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
+    <workbookView xWindow="5385" yWindow="720" windowWidth="21165" windowHeight="14865" xr2:uid="{3EAF054D-113C-4C08-8374-C110A2D9B948}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Category</t>
   </si>
@@ -55,6 +55,15 @@
   <si>
     <t>Python strings have several methods to check for their type of contents. 1. Find logic in the problem. Palindromes read the same both ways, reverse the string.
 2. Start a pointer at each side of the string, use an alphanumeric validation function, and move the pointers if they are not alphanumeric.</t>
+  </si>
+  <si>
+    <t>Arrays and Hashing</t>
+  </si>
+  <si>
+    <t>271 - Encode and Decode String</t>
+  </si>
+  <si>
+    <t>Encode strings using an int to signal the length and use a special character to know when to start the counting.</t>
   </si>
 </sst>
 </file>
@@ -70,7 +79,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +89,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,7 +111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -110,6 +125,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,16 +460,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041B7148-3DCA-4078-893C-34A3490F6593}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="138.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -479,6 +495,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>